<commit_message>
Guia M1 sin soluciones
</commit_message>
<xml_diff>
--- a/P101.xlsx
+++ b/P101.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dragonnomada/Desktop/banjercito/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3B9D40-782B-964B-80A8-6C386E7B40D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8363A96D-C430-1A46-BEA3-219A41712460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="31840" windowHeight="17440" xr2:uid="{1EC4F91A-27D7-F143-9E1E-71D977924F0D}"/>
+    <workbookView xWindow="5180" yWindow="1800" windowWidth="32980" windowHeight="17440" activeTab="1" xr2:uid="{1EC4F91A-27D7-F143-9E1E-71D977924F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Solución" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>Cliente</t>
   </si>
@@ -215,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -227,14 +228,13 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6C4568-CC50-3540-AD1A-CAB7CB90CF78}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="191" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,13 +597,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -702,13 +702,13 @@
       <c r="D6" s="5">
         <v>3200</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -725,50 +725,49 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F8" s="9" t="s">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="10" t="str" cm="1">
+      <c r="G8" t="str" cm="1">
         <f t="array" ref="G8:J10">_xlfn._xlws.FILTER(A2:D7,B2:B7=F3)</f>
         <v>C001</v>
       </c>
-      <c r="H8" s="10" t="str">
+      <c r="H8" t="str">
         <v>Hombre</v>
       </c>
-      <c r="I8" s="10" t="str">
+      <c r="I8" t="str">
         <v>P0001</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <v>14600</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F9" s="10"/>
-      <c r="G9" s="10" t="str">
+      <c r="G9" t="str">
         <v>C003</v>
       </c>
-      <c r="H9" s="10" t="str">
+      <c r="H9" t="str">
         <v>Hombre</v>
       </c>
-      <c r="I9" s="10" t="str">
+      <c r="I9" t="str">
         <v>E0004</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <v>12000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="str">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="str">
         <v>C006</v>
       </c>
-      <c r="H10" s="12" t="str">
+      <c r="H10" s="10" t="str">
         <v>Hombre</v>
       </c>
-      <c r="I10" s="12" t="str">
+      <c r="I10" s="10" t="str">
         <v>G0128</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="11">
         <v>23700</v>
       </c>
     </row>
@@ -779,50 +778,49 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F13" s="10" t="s">
+      <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="10" t="str" cm="1">
+      <c r="G13" t="str" cm="1">
         <f t="array" ref="G13:J15">_xlfn._xlws.FILTER(A2:D7, B2:B7=F4)</f>
         <v>C002</v>
       </c>
-      <c r="H13" s="10" t="str">
+      <c r="H13" t="str">
         <v>Mujer</v>
       </c>
-      <c r="I13" s="10" t="str">
+      <c r="I13" t="str">
         <v>P0002</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <v>18900</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="str">
+      <c r="G14" t="str">
         <v>C004</v>
       </c>
-      <c r="H14" s="10" t="str">
+      <c r="H14" t="str">
         <v>Mujer</v>
       </c>
-      <c r="I14" s="10" t="str">
+      <c r="I14" t="str">
         <v>E0032</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="9">
         <v>6900</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F15" s="12"/>
-      <c r="G15" s="12" t="str">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="str">
         <v>C005</v>
       </c>
-      <c r="H15" s="12" t="str">
+      <c r="H15" s="10" t="str">
         <v>Mujer</v>
       </c>
-      <c r="I15" s="12" t="str">
+      <c r="I15" s="10" t="str">
         <v>F0005</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="11">
         <v>3200</v>
       </c>
     </row>
@@ -839,4 +837,244 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69925B7-F0BF-6A42-BD2D-67E29B08D341}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="230" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <v>14600</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <f>SUMIF(B2:B7,"Hombre",D2:D7)</f>
+        <v>50300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>18900</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f>SUMIF(B2:B7,"Mujer",D2:D7)</f>
+        <v>29000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6900</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" ref="G5:J7">_xlfn._xlws.FILTER(A2:D7,B2:B7="Hombre")</f>
+        <v>C001</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Hombre</v>
+      </c>
+      <c r="I5" t="str">
+        <v>P0001</v>
+      </c>
+      <c r="J5">
+        <v>14600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3200</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="str">
+        <v>C003</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Hombre</v>
+      </c>
+      <c r="I6" t="str">
+        <v>E0004</v>
+      </c>
+      <c r="J6">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <v>23700</v>
+      </c>
+      <c r="G7" t="str">
+        <v>C006</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Hombre</v>
+      </c>
+      <c r="I7" t="str">
+        <v>G0128</v>
+      </c>
+      <c r="J7">
+        <v>23700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" t="str" cm="1">
+        <f t="array" ref="D10:D15">B2:B7</f>
+        <v>Hombre</v>
+      </c>
+      <c r="E10" s="13" t="b" cm="1">
+        <f t="array" ref="E10:E15">B2:B7="Hombre"</f>
+        <v>1</v>
+      </c>
+      <c r="G10" cm="1">
+        <f t="array" ref="G10:G12">_xlfn._xlws.FILTER(D2:D7,B2:B7="Mujer")</f>
+        <v>18900</v>
+      </c>
+      <c r="I10" s="1" cm="1">
+        <f t="array" ref="I10">SUM(_xlfn._xlws.FILTER(D2:D7,B2:B7="Hombre"))</f>
+        <v>50300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" t="str">
+        <v>Mujer</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D12" t="str">
+        <v>Hombre</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D13" t="str">
+        <v>Mujer</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D14" t="str">
+        <v>Mujer</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D15" t="str">
+        <v>Hombre</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>